<commit_message>
tdf#89139 Fix exporting of DateTime to CacheDefinition according to ISO 8601
Change-Id: I1239f5582173afe99bf9178fd4edd1dc5ca28e8e
</commit_message>
<xml_diff>
--- a/sc/qa/unit/data/xlsx/pivot.xlsx
+++ b/sc/qa/unit/data/xlsx/pivot.xlsx
@@ -1,94 +1,92 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28502"/>
-  <workbookPr hidePivotFieldList="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18509"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/NavKit/Downloads/pivotcache-files/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2091187C-1A30-45A4-A52A-DF2E0150E7E5}" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="18260" windowHeight="14460"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="18260" windowHeight="14460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet5" sheetId="7" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="SheetWithPivot" sheetId="7" r:id="rId1"/>
+    <sheet name="SheetWithData" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="171026" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="45" r:id="rId3"/>
+    <pivotCache cacheId="7030" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
-  <si>
-    <t>imieinazwisko</t>
-  </si>
-  <si>
-    <t>wartosc</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Sum of druga wartosc</t>
   </si>
   <si>
     <t>bartosz</t>
   </si>
   <si>
-    <t>Row Labels</t>
+    <t>grzegorz</t>
+  </si>
+  <si>
+    <t>kosiorek</t>
+  </si>
+  <si>
+    <t>maciej</t>
+  </si>
+  <si>
+    <t>(blank)</t>
   </si>
   <si>
     <t>Grand Total</t>
   </si>
   <si>
-    <t>(blank)</t>
-  </si>
-  <si>
-    <t>kosiorek</t>
-  </si>
-  <si>
-    <t>druga wartosc</t>
-  </si>
-  <si>
-    <t>trzecia wartosc</t>
+    <t>mixed strings and empty</t>
+  </si>
+  <si>
+    <t>mixed empty fileds and integers</t>
+  </si>
+  <si>
+    <t>all fields are integers</t>
+  </si>
+  <si>
+    <t>mixed strings and integers</t>
+  </si>
+  <si>
+    <t>date and time with duplicated entries</t>
   </si>
   <si>
     <t>tekst</t>
-  </si>
-  <si>
-    <t>grzegorz</t>
-  </si>
-  <si>
-    <t>maciej</t>
-  </si>
-  <si>
-    <t>czwarta wartosc</t>
-  </si>
-  <si>
-    <t>tekscik</t>
-  </si>
-  <si>
-    <t>tekscik2</t>
-  </si>
-  <si>
-    <t>Sum of druga wartosc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
+  </numFmts>
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,13 +115,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -142,9 +141,9 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Microsoft Office User" refreshedDate="42950.628587384257" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="5">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Excel Services" refreshedDate="42961.916244791668" createdVersion="4" refreshedVersion="6" minRefreshableVersion="3" recordCount="5" xr:uid="{00000000-000A-0000-FFFF-FFFF2D000000}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A2:E7" sheet="Sheet1"/>
+    <worksheetSource ref="A2:E7" sheet="SheetWithData"/>
   </cacheSource>
   <cacheFields count="5">
     <cacheField name="imieinazwisko" numFmtId="0">
@@ -157,11 +156,7 @@
       </sharedItems>
     </cacheField>
     <cacheField name="wartosc" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="111" maxValue="222" count="3">
-        <m/>
-        <n v="111"/>
-        <n v="222"/>
-      </sharedItems>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="111" maxValue="222"/>
     </cacheField>
     <cacheField name="druga wartosc" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1111" maxValue="5555"/>
@@ -169,8 +164,8 @@
     <cacheField name="trzecia wartosc" numFmtId="0">
       <sharedItems containsMixedTypes="1" containsNumber="1" containsInteger="1" minValue="1234" maxValue="5678"/>
     </cacheField>
-    <cacheField name="czwarta wartosc" numFmtId="0">
-      <sharedItems containsBlank="1" containsMixedTypes="1" containsNumber="1" containsInteger="1" minValue="11" maxValue="22"/>
+    <cacheField name="date and time" numFmtId="164">
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="1903-08-24T07:40:48" maxDate="2024-05-23T07:12:00"/>
     </cacheField>
   </cacheFields>
   <extLst>
@@ -182,47 +177,47 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="5">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="5">
   <r>
     <x v="0"/>
-    <x v="0"/>
+    <m/>
     <n v="1111"/>
     <n v="2345"/>
-    <m/>
+    <d v="1982-02-18T15:36:00"/>
   </r>
   <r>
     <x v="1"/>
-    <x v="1"/>
+    <n v="111"/>
     <n v="2222"/>
     <s v="tekst"/>
-    <s v="tekscik"/>
+    <d v="2024-05-23T07:12:00"/>
   </r>
   <r>
     <x v="2"/>
-    <x v="2"/>
+    <n v="222"/>
     <n v="3333"/>
     <n v="1234"/>
-    <n v="11"/>
+    <d v="1903-08-24T07:40:48"/>
   </r>
   <r>
     <x v="3"/>
-    <x v="0"/>
+    <m/>
     <n v="4444"/>
     <s v="tekst"/>
-    <s v="tekscik2"/>
+    <d v="1911-11-21T07:59:31"/>
   </r>
   <r>
     <x v="4"/>
-    <x v="0"/>
+    <m/>
     <n v="5555"/>
     <n v="5678"/>
-    <n v="22"/>
+    <d v="1936-03-23T04:48:00"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="45" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable4" cacheId="7030" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" showAll="0">
@@ -235,17 +230,10 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="1"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
+    <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
     <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
   </pivotFields>
   <rowFields count="1">
     <field x="0"/>
@@ -280,6 +268,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
     </ext>
   </extLst>
 </pivotTableDefinition>
@@ -547,31 +538,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" customWidth="1"/>
-    <col min="3" max="3" width="4.1640625" customWidth="1"/>
-    <col min="4" max="4" width="6.5" customWidth="1"/>
-    <col min="5" max="5" width="10" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -579,41 +568,41 @@
         <v>2222</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B5" s="3">
         <v>5555</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B6" s="3">
         <v>4444</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B7" s="3">
         <v>1111</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B8" s="3">
         <v>3333</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B9" s="3">
         <v>16665</v>
@@ -625,38 +614,39 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.1640625" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C3">
         <v>1111</v>
@@ -664,8 +654,11 @@
       <c r="D3">
         <v>2345</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E3" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -676,13 +669,13 @@
         <v>2222</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E4" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="B5">
         <v>222</v>
       </c>
@@ -692,27 +685,27 @@
       <c r="D5">
         <v>1234</v>
       </c>
-      <c r="E5">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E5" s="4">
+        <v>30000.67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C6">
         <v>4444</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="E6" s="4">
+        <v>40000.453500000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C7">
         <v>5555</v>
@@ -720,8 +713,8 @@
       <c r="D7">
         <v>5678</v>
       </c>
-      <c r="E7">
-        <v>22</v>
+      <c r="E7" s="4">
+        <v>13232.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>